<commit_message>
fixed sideways nfets, relayed out the area around the new FET configuration. BOM updates for all the initial parts.  BOM reflects the fixed NFET pinout.
</commit_message>
<xml_diff>
--- a/photon-base-pcb/goldentee-topper-base.xlsx
+++ b/photon-base-pcb/goldentee-topper-base.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28016"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leste\Documents\goldenteetopper-photon\photon-base-pcb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lestermeeks/Documents/Projects/git/goldenteetopper-photon/photon-base-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="5560" yWindow="3660" windowWidth="24620" windowHeight="13580"/>
   </bookViews>
   <sheets>
     <sheet name="goldentee-topper-base" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
   <si>
     <t>Reference</t>
   </si>
@@ -169,16 +177,94 @@
   </si>
   <si>
     <t>1276-1854-1-ND</t>
+  </si>
+  <si>
+    <t>A1972-ND</t>
+  </si>
+  <si>
+    <t>TE/AMP</t>
+  </si>
+  <si>
+    <t>640445-4</t>
+  </si>
+  <si>
+    <t>1-640445-6</t>
+  </si>
+  <si>
+    <t>1-640445-6-ND</t>
+  </si>
+  <si>
+    <t>Amphenol</t>
+  </si>
+  <si>
+    <t>68000-406HLF</t>
+  </si>
+  <si>
+    <t>609-3263-ND</t>
+  </si>
+  <si>
+    <t>CL21B103KAANNNC</t>
+  </si>
+  <si>
+    <t>1276-2434-1-ND</t>
+  </si>
+  <si>
+    <t>Fairchild/ON Semi</t>
+  </si>
+  <si>
+    <t>BSS138LCT-ND</t>
+  </si>
+  <si>
+    <t>NOT SOIC WRONG FP</t>
+  </si>
+  <si>
+    <t>NEED A GSD pinout</t>
+  </si>
+  <si>
+    <t>BSS138L</t>
+  </si>
+  <si>
+    <t>Diodes Inc</t>
+  </si>
+  <si>
+    <t>DMP3010LK3-13</t>
+  </si>
+  <si>
+    <t>DMP3010LK3-13DICT-ND</t>
+  </si>
+  <si>
+    <t>NCP1117ST50T3GOSCT-ND</t>
+  </si>
+  <si>
+    <t>On Semi</t>
+  </si>
+  <si>
+    <t>NCP1117ST50T3G</t>
+  </si>
+  <si>
+    <t>SN74LVC2T45DCTR</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>296-16845-1-ND</t>
+  </si>
+  <si>
+    <t>particle.io</t>
+  </si>
+  <si>
+    <t>photon dev module</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +395,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -656,9 +748,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1015,26 +1111,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1162,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1079,13 +1175,27 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1">
+        <v>0.26</v>
+      </c>
       <c r="F2" s="1">
         <f t="shared" ref="F2:F4" si="0">E2*D2</f>
-        <v>0</v>
+        <v>0.26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1098,13 +1208,27 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1">
+        <v>1.01</v>
+      </c>
       <c r="F3" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.01</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1117,13 +1241,27 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <v>0.25</v>
+      </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1137,11 +1275,11 @@
         <v>26</v>
       </c>
       <c r="E5" s="1">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="F5" s="1">
         <f>E5*D5</f>
-        <v>2.6</v>
+        <v>0.52</v>
       </c>
       <c r="G5" t="s">
         <v>43</v>
@@ -1156,7 +1294,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1170,11 +1308,11 @@
         <v>2</v>
       </c>
       <c r="E6" s="1">
-        <v>0.24</v>
+        <v>0.03</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" ref="F6:F12" si="1">E6*D6</f>
-        <v>0.48</v>
+        <v>0.06</v>
       </c>
       <c r="G6" t="s">
         <v>47</v>
@@ -1189,26 +1327,43 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1">
+      <c r="E7" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.59</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1221,32 +1376,63 @@
       <c r="D8">
         <v>6</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>0.02</v>
+      </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>0.19</v>
+      </c>
       <c r="F9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1259,13 +1445,27 @@
       <c r="D10">
         <v>7</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="F10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.9200000000000004</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1283,8 +1483,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="G11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1297,10 +1503,30 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>0.39</v>
+      </c>
       <c r="F12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.39</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F13" s="4">
+        <f>SUM(F2:F12)</f>
+        <v>9.4500000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pre level shifter and nchan fix.
</commit_message>
<xml_diff>
--- a/photon-base-pcb/goldentee-topper-base.xlsx
+++ b/photon-base-pcb/goldentee-topper-base.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="3660" windowWidth="24620" windowHeight="13580"/>
+    <workbookView xWindow="-27280" yWindow="3680" windowWidth="24620" windowHeight="13580"/>
   </bookViews>
   <sheets>
     <sheet name="goldentee-topper-base" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>SN74LVC2T45</t>
   </si>
   <si>
-    <t>SMD_Packages:SOIC-8-N</t>
-  </si>
-  <si>
     <t>0.1uF 25V</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>photon dev module</t>
+  </si>
+  <si>
+    <t>goldentee_topper_base:SN74LVC2T45DCTR</t>
   </si>
 </sst>
 </file>
@@ -748,13 +748,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1114,7 +1113,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1141,25 +1140,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
       <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1183,16 +1182,16 @@
         <v>0.26</v>
       </c>
       <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
         <v>51</v>
       </c>
-      <c r="H2" t="s">
-        <v>52</v>
-      </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1216,27 +1215,27 @@
         <v>1.01</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
         <v>53</v>
-      </c>
-      <c r="I3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1249,21 +1248,21 @@
         <v>0.25</v>
       </c>
       <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s">
         <v>55</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
         <v>56</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -1282,21 +1281,21 @@
         <v>0.52</v>
       </c>
       <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
         <v>43</v>
       </c>
-      <c r="H5" t="s">
-        <v>44</v>
-      </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1315,63 +1314,63 @@
         <v>0.06</v>
       </c>
       <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s">
         <v>47</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" t="s">
         <v>48</v>
       </c>
-      <c r="I6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" t="s">
-        <v>49</v>
-      </c>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>0.53</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <f t="shared" si="1"/>
         <v>1.59</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>62</v>
+      <c r="K7" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1384,63 +1383,63 @@
         <v>0.12</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" t="s">
         <v>58</v>
       </c>
-      <c r="I8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" t="s">
-        <v>59</v>
-      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>7</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>0.19</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="4">
         <f t="shared" si="1"/>
         <v>1.33</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H9" t="s">
-        <v>64</v>
-      </c>
-      <c r="I9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" t="s">
-        <v>61</v>
-      </c>
-      <c r="K9" t="s">
-        <v>63</v>
+      <c r="K9" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -1453,27 +1452,27 @@
         <v>3.9200000000000004</v>
       </c>
       <c r="G10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" t="s">
         <v>65</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" t="s">
         <v>66</v>
-      </c>
-      <c r="I10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1484,21 +1483,21 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" t="s">
         <v>74</v>
-      </c>
-      <c r="H11" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1511,20 +1510,20 @@
         <v>0.39</v>
       </c>
       <c r="G12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" t="s">
         <v>69</v>
       </c>
-      <c r="H12" t="s">
-        <v>70</v>
-      </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F13" s="4">
+      <c r="F13" s="2">
         <f>SUM(F2:F12)</f>
         <v>9.4500000000000011</v>
       </c>

</xml_diff>